<commit_message>
adding to the diary #1
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cookd/teaching/ETC5521/eda-private/assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Uni work monash ver\ETC5521\Asm 3 group\assignment-3-acdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E6E8D6-D05B-C146-B3DA-2457C8448439}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE58713E-2B9A-46FA-B51C-FCE9D452CDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="820" windowWidth="27860" windowHeight="16940" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Team Name:</t>
   </si>
@@ -72,12 +72,24 @@
 Fix merge conflict 
 Decide on choice of methods for first part</t>
   </si>
+  <si>
+    <t>acdc</t>
+  </si>
+  <si>
+    <t>mpha0054</t>
+  </si>
+  <si>
+    <t>kngu0086</t>
+  </si>
+  <si>
+    <t>Choosing the topic for the assignment and deciding on workflow.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,6 +120,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -129,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -142,6 +160,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,37 +475,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.69921875" customWidth="1"/>
+    <col min="5" max="5" width="38.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -503,7 +531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45183</v>
       </c>
@@ -520,12 +548,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="10" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45186</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating the diary for 02/10/2023
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Uni work monash ver\ETC5521\Asm 3 group\assignment-3-acdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE58713E-2B9A-46FA-B51C-FCE9D452CDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8981B2-B5D7-4652-8B71-BDC9CF5C90EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Team Name:</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Choosing the topic for the assignment and deciding on workflow.</t>
+  </si>
+  <si>
+    <t>Fixing expectations and deciding on how to proceed with the weather data</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -570,6 +573,23 @@
         <v>14</v>
       </c>
     </row>
+    <row r="12" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45201</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Final touches on the dairy and script
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kelly/Desktop/ETC5521 - Exploratory Data Analysis/Assignments/Assignment3/assignment-3-acdc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Uni work monash ver\ETC5521\Asm 3 group\assignment-3-acdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A185DC-276C-3347-B7E7-7FE3469E7E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8917D28-6D06-4182-BD91-A47869649A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Team Name:</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t>Merging branches, dicussing next steps</t>
+  </si>
+  <si>
+    <t>Discussing temperature data and what to plot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalize the report and fixing aesthestics </t>
   </si>
 </sst>
 </file>
@@ -482,19 +491,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.69921875" customWidth="1"/>
+    <col min="5" max="5" width="38.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -513,15 +522,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -538,7 +547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45183</v>
       </c>
@@ -555,12 +564,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45186</v>
       </c>
@@ -577,7 +586,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45201</v>
       </c>
@@ -594,7 +603,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45202</v>
       </c>
@@ -609,6 +618,40 @@
       </c>
       <c r="E14" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45204</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>45205</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.6875</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating the team diary
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Uni work monash ver\ETC5521\Asm 3 group\assignment-3-acdc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhajena/Downloads/semester2/ETC5521/assignment-3-acdc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8917D28-6D06-4182-BD91-A47869649A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB83905-D243-2E4D-B8C0-381919F81A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Team Name:</t>
   </si>
@@ -98,6 +99,12 @@
   </si>
   <si>
     <t xml:space="preserve">Finalize the report and fixing aesthestics </t>
+  </si>
+  <si>
+    <t>Evan,Amrita,Phuong Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First team meeting completed - disucussing the action plan to proceed further </t>
   </si>
 </sst>
 </file>
@@ -493,17 +500,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.69921875" customWidth="1"/>
-    <col min="5" max="5" width="38.296875" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -522,15 +529,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -547,7 +554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="78" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45183</v>
       </c>
@@ -564,12 +571,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45186</v>
       </c>
@@ -586,7 +593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45201</v>
       </c>
@@ -603,7 +610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>45202</v>
       </c>
@@ -620,7 +627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>45204</v>
       </c>
@@ -637,7 +644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>45205</v>
       </c>
@@ -658,4 +665,117 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987BD012-24AF-D84B-99DB-8D8570822A35}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>45183</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Amended the meeting diary
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhajena/Downloads/semester2/ETC5521/assignment-3-acdc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evang\Documents\Monash University\Semester 2\ETC5521\Assignment\Assignment 4\assignment-3-acdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB83905-D243-2E4D-B8C0-381919F81A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF263DEF-F1D0-4B70-934A-C0B1E5BD7078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Team Name:</t>
   </si>
@@ -101,10 +103,17 @@
     <t xml:space="preserve">Finalize the report and fixing aesthestics </t>
   </si>
   <si>
-    <t>Evan,Amrita,Phuong Mai</t>
-  </si>
-  <si>
     <t xml:space="preserve">First team meeting completed - disucussing the action plan to proceed further </t>
+  </si>
+  <si>
+    <t>- All
+- Previous Team</t>
+  </si>
+  <si>
+    <t>Getting insights from the previous team who handle the wild sighting</t>
+  </si>
+  <si>
+    <t>Evan, Amrita, Phuong Mai</t>
   </si>
 </sst>
 </file>
@@ -169,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -184,6 +193,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,13 +516,13 @@
       <selection sqref="A1:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
     <col min="5" max="5" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -529,15 +541,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -554,7 +566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45183</v>
       </c>
@@ -571,12 +583,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45186</v>
       </c>
@@ -593,7 +605,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45201</v>
       </c>
@@ -610,7 +622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45202</v>
       </c>
@@ -627,7 +639,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45204</v>
       </c>
@@ -644,7 +656,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45205</v>
       </c>
@@ -672,10 +684,10 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
@@ -684,7 +696,7 @@
     <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,24 +704,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C2" s="8"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -726,9 +738,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>45183</v>
+        <v>45213</v>
       </c>
       <c r="B7" s="3">
         <v>0.42708333333333331</v>
@@ -740,37 +752,49 @@
         <v>7</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>45215</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>

</xml_diff>

<commit_message>
Updating group diary 24/10
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhajena/Downloads/semester2/ETC5521/assignment-3-acdc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phuongann/Monash/Ms of Business Analytics_S12023/ETC5521/assignment-3-acdc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797282BC-8B2E-7B43-BEDD-D30F0C17F37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019EF06C-E98B-C044-A6E4-4251C042DD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16440" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Team Name:</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Working on the temporal and eco tourism analysis</t>
+  </si>
+  <si>
+    <t>Checking on the working process of groups member and discussing about the presentations and adjustments. Assigning editing tasks.</t>
   </si>
 </sst>
 </file>
@@ -687,7 +690,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -792,11 +795,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="E10" s="6"/>
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>45223</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>

</xml_diff>

<commit_message>
updating the group diary
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phuongann/Monash/Ms of Business Analytics_S12023/ETC5521/assignment-3-acdc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhajena/Downloads/semester2/ETC5521/assignment-3-acdc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019EF06C-E98B-C044-A6E4-4251C042DD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3958C9DC-7741-DA4E-AF36-1272F3355E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16440" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16140" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Team Name:</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Checking on the working process of groups member and discussing about the presentations and adjustments. Assigning editing tasks.</t>
+  </si>
+  <si>
+    <t>Preparing for the presentation and checking the final report.</t>
   </si>
 </sst>
 </file>
@@ -690,7 +693,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,7 +702,7 @@
     <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -812,6 +815,23 @@
         <v>25</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>45225</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>

</xml_diff>

<commit_message>
Ammended Diary Meeting for Octiber 27th, 2023
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhajena/Downloads/semester2/ETC5521/assignment-3-acdc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evang\Documents\Monash University\Semester 2\ETC5521\Assignment\Assignment 4\assignment-3-acdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3958C9DC-7741-DA4E-AF36-1272F3355E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B6586E-6ED3-47B6-AA64-3A633AB74A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16140" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Team Name:</t>
   </si>
@@ -123,6 +123,16 @@
   </si>
   <si>
     <t>Preparing for the presentation and checking the final report.</t>
+  </si>
+  <si>
+    <t>Second preparation for the video presentation</t>
+  </si>
+  <si>
+    <t>- ACDC Team
+- INSX Team</t>
+  </si>
+  <si>
+    <t>Making Video Presentation</t>
   </si>
 </sst>
 </file>
@@ -187,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -204,6 +214,21 @@
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,13 +550,13 @@
       <selection sqref="A1:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
     <col min="5" max="5" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -550,15 +575,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -575,7 +600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45183</v>
       </c>
@@ -592,12 +617,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45186</v>
       </c>
@@ -614,7 +639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45201</v>
       </c>
@@ -631,7 +656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45202</v>
       </c>
@@ -648,7 +673,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45204</v>
       </c>
@@ -665,7 +690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45205</v>
       </c>
@@ -692,11 +717,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987BD012-24AF-D84B-99DB-8D8570822A35}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
@@ -705,7 +730,7 @@
     <col min="5" max="5" width="50.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +738,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -722,15 +747,15 @@
       </c>
       <c r="C2" s="8"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -747,7 +772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45213</v>
       </c>
@@ -764,7 +789,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45215</v>
       </c>
@@ -781,7 +806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45218</v>
       </c>
@@ -798,57 +823,85 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
         <v>45223</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="12">
         <v>0.39583333333333331</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
         <v>45225</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B11" s="12">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="11">
+        <v>45226</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A13" s="11">
+        <v>45226</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0.4375</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.46875</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>

</xml_diff>